<commit_message>
lectura de datos realizado
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7875" windowWidth="15300" xWindow="23280" yWindow="1050"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,17 +51,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -428,14 +427,14 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="1" width="10.7109375"/>
-    <col customWidth="1" max="6" min="6" style="1" width="13.85546875"/>
-    <col customWidth="1" max="7" min="7" style="1" width="17.28515625"/>
-    <col customWidth="1" max="9" min="9" style="1" width="11.28515625"/>
-    <col customWidth="1" max="10" min="10" style="1" width="8.85546875"/>
-    <col customWidth="1" max="11" min="11" style="1" width="24.5703125"/>
+    <col width="10.6640625" customWidth="1" min="2" max="2"/>
+    <col width="13.88671875" customWidth="1" min="6" max="6"/>
+    <col width="17.33203125" customWidth="1" min="7" max="7"/>
+    <col width="11.33203125" customWidth="1" min="9" max="9"/>
+    <col width="8.88671875" customWidth="1" min="10" max="10"/>
+    <col width="24.5546875" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -628,7 +627,7 @@
       <c r="I5" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="2" t="n"/>
+      <c r="K5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -759,6 +758,9 @@
           <t>David</t>
         </is>
       </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Danza</t>
@@ -772,10 +774,33 @@
       </c>
     </row>
     <row r="10">
-      <c r="M10" s="2" t="n"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Lopez</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Mendoza</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Tania</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Guadalupe</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>